<commit_message>
add new dataset frame
</commit_message>
<xml_diff>
--- a/PROJECT DATASET.xlsx
+++ b/PROJECT DATASET.xlsx
@@ -843,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -854,28 +854,28 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
@@ -930,9 +930,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="17" applyFont="1" fillId="0" applyAlignment="1">
@@ -1258,17 +1255,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="40.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="32" width="62.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="33" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="33" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="32" width="8.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="34" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="35" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="31" width="40.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="31" width="62.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="32" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="32" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="31" width="8.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="34" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="31" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="31" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="31" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="31" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1481,7 +1478,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="1057.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="306">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -2145,13 +2142,13 @@
       <c r="D42" s="29">
         <v>12</v>
       </c>
-      <c r="E42" s="30"/>
+      <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="7" t="s">
@@ -2166,13 +2163,13 @@
       <c r="D43" s="29">
         <v>104</v>
       </c>
-      <c r="E43" s="30"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="5"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="7" t="s">
@@ -2187,13 +2184,13 @@
       <c r="D44" s="29">
         <v>170</v>
       </c>
-      <c r="E44" s="30"/>
+      <c r="E44" s="4"/>
       <c r="F44" s="5"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="7" t="s">
@@ -2208,13 +2205,13 @@
       <c r="D45" s="29">
         <v>33</v>
       </c>
-      <c r="E45" s="30"/>
+      <c r="E45" s="4"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="7" t="s">
@@ -2229,13 +2226,13 @@
       <c r="D46" s="29">
         <v>9</v>
       </c>
-      <c r="E46" s="30"/>
+      <c r="E46" s="4"/>
       <c r="F46" s="5"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="7" t="s">
@@ -2250,13 +2247,13 @@
       <c r="D47" s="29">
         <v>49</v>
       </c>
-      <c r="E47" s="30"/>
+      <c r="E47" s="4"/>
       <c r="F47" s="5"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="7" t="s">
@@ -2271,13 +2268,13 @@
       <c r="D48" s="29">
         <v>63</v>
       </c>
-      <c r="E48" s="30"/>
+      <c r="E48" s="4"/>
       <c r="F48" s="5"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="7" t="s">
@@ -2292,13 +2289,13 @@
       <c r="D49" s="29">
         <v>43</v>
       </c>
-      <c r="E49" s="30"/>
+      <c r="E49" s="4"/>
       <c r="F49" s="5"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="7" t="s">
@@ -2313,13 +2310,13 @@
       <c r="D50" s="29">
         <v>21</v>
       </c>
-      <c r="E50" s="30"/>
+      <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="7" t="s">
@@ -2334,13 +2331,13 @@
       <c r="D51" s="29">
         <v>413</v>
       </c>
-      <c r="E51" s="30"/>
+      <c r="E51" s="4"/>
       <c r="F51" s="5"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="7" t="s">
@@ -2355,13 +2352,13 @@
       <c r="D52" s="29">
         <v>37</v>
       </c>
-      <c r="E52" s="30"/>
+      <c r="E52" s="4"/>
       <c r="F52" s="5"/>
       <c r="G52" s="6"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="7" t="s">
@@ -2376,13 +2373,13 @@
       <c r="D53" s="29">
         <v>335</v>
       </c>
-      <c r="E53" s="30"/>
+      <c r="E53" s="4"/>
       <c r="F53" s="5"/>
       <c r="G53" s="6"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="7" t="s">
@@ -2397,13 +2394,13 @@
       <c r="D54" s="29">
         <v>136</v>
       </c>
-      <c r="E54" s="30"/>
+      <c r="E54" s="4"/>
       <c r="F54" s="5"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="7" t="s">
@@ -2418,13 +2415,13 @@
       <c r="D55" s="29">
         <v>98</v>
       </c>
-      <c r="E55" s="30"/>
+      <c r="E55" s="4"/>
       <c r="F55" s="5"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="7" t="s">
@@ -2439,13 +2436,13 @@
       <c r="D56" s="29">
         <v>45</v>
       </c>
-      <c r="E56" s="30"/>
+      <c r="E56" s="4"/>
       <c r="F56" s="5"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
-      <c r="J56" s="30"/>
-      <c r="K56" s="30"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="7" t="s">
@@ -2460,13 +2457,13 @@
       <c r="D57" s="29">
         <v>910</v>
       </c>
-      <c r="E57" s="30"/>
+      <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="6"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="7" t="s">
@@ -2481,13 +2478,13 @@
       <c r="D58" s="29">
         <v>372</v>
       </c>
-      <c r="E58" s="30"/>
+      <c r="E58" s="4"/>
       <c r="F58" s="5"/>
       <c r="G58" s="6"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="30"/>
-      <c r="J58" s="30"/>
-      <c r="K58" s="30"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="7" t="s">
@@ -2502,13 +2499,13 @@
       <c r="D59" s="29">
         <v>82</v>
       </c>
-      <c r="E59" s="30"/>
+      <c r="E59" s="4"/>
       <c r="F59" s="5"/>
       <c r="G59" s="6"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="7" t="s">
@@ -2523,13 +2520,13 @@
       <c r="D60" s="29">
         <v>41</v>
       </c>
-      <c r="E60" s="30"/>
+      <c r="E60" s="4"/>
       <c r="F60" s="5"/>
       <c r="G60" s="6"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="7" t="s">
@@ -2544,13 +2541,13 @@
       <c r="D61" s="29">
         <v>301</v>
       </c>
-      <c r="E61" s="30"/>
+      <c r="E61" s="4"/>
       <c r="F61" s="5"/>
       <c r="G61" s="6"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="7" t="s">
@@ -2565,13 +2562,13 @@
       <c r="D62" s="29">
         <v>47</v>
       </c>
-      <c r="E62" s="30"/>
+      <c r="E62" s="4"/>
       <c r="F62" s="5"/>
       <c r="G62" s="6"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="30"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="7" t="s">
@@ -2586,13 +2583,13 @@
       <c r="D63" s="29">
         <v>117</v>
       </c>
-      <c r="E63" s="30"/>
+      <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="6"/>
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
-      <c r="J63" s="30"/>
-      <c r="K63" s="30"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="7" t="s">
@@ -2607,13 +2604,13 @@
       <c r="D64" s="29">
         <v>814</v>
       </c>
-      <c r="E64" s="30"/>
+      <c r="E64" s="4"/>
       <c r="F64" s="5"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="7" t="s">
@@ -2628,13 +2625,13 @@
       <c r="D65" s="29">
         <v>205</v>
       </c>
-      <c r="E65" s="30"/>
+      <c r="E65" s="4"/>
       <c r="F65" s="5"/>
       <c r="G65" s="6"/>
-      <c r="H65" s="30"/>
-      <c r="I65" s="30"/>
-      <c r="J65" s="30"/>
-      <c r="K65" s="30"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="7" t="s">
@@ -2649,13 +2646,13 @@
       <c r="D66" s="29">
         <v>38</v>
       </c>
-      <c r="E66" s="30"/>
+      <c r="E66" s="4"/>
       <c r="F66" s="5"/>
       <c r="G66" s="6"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="30"/>
-      <c r="J66" s="30"/>
-      <c r="K66" s="30"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="7" t="s">
@@ -2670,13 +2667,13 @@
       <c r="D67" s="29">
         <v>571</v>
       </c>
-      <c r="E67" s="30"/>
+      <c r="E67" s="4"/>
       <c r="F67" s="5"/>
       <c r="G67" s="6"/>
-      <c r="H67" s="30"/>
-      <c r="I67" s="30"/>
-      <c r="J67" s="30"/>
-      <c r="K67" s="30"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="7" t="s">
@@ -2691,13 +2688,13 @@
       <c r="D68" s="29">
         <v>963</v>
       </c>
-      <c r="E68" s="30"/>
+      <c r="E68" s="4"/>
       <c r="F68" s="5"/>
       <c r="G68" s="6"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="30"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="7" t="s">
@@ -2712,13 +2709,13 @@
       <c r="D69" s="29">
         <v>22</v>
       </c>
-      <c r="E69" s="30"/>
+      <c r="E69" s="4"/>
       <c r="F69" s="5"/>
       <c r="G69" s="6"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="7" t="s">
@@ -2733,13 +2730,13 @@
       <c r="D70" s="29">
         <v>24</v>
       </c>
-      <c r="E70" s="30"/>
+      <c r="E70" s="4"/>
       <c r="F70" s="5"/>
       <c r="G70" s="6"/>
-      <c r="H70" s="30"/>
-      <c r="I70" s="30"/>
-      <c r="J70" s="30"/>
-      <c r="K70" s="30"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="7" t="s">
@@ -2754,13 +2751,13 @@
       <c r="D71" s="29">
         <v>24</v>
       </c>
-      <c r="E71" s="30"/>
+      <c r="E71" s="4"/>
       <c r="F71" s="5"/>
       <c r="G71" s="6"/>
-      <c r="H71" s="30"/>
-      <c r="I71" s="30"/>
-      <c r="J71" s="30"/>
-      <c r="K71" s="30"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="7" t="s">
@@ -2775,13 +2772,13 @@
       <c r="D72" s="29">
         <v>55</v>
       </c>
-      <c r="E72" s="30"/>
+      <c r="E72" s="4"/>
       <c r="F72" s="5"/>
       <c r="G72" s="6"/>
-      <c r="H72" s="30"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30"/>
-      <c r="K72" s="30"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="7" t="s">
@@ -2796,13 +2793,13 @@
       <c r="D73" s="29">
         <v>51</v>
       </c>
-      <c r="E73" s="30"/>
+      <c r="E73" s="4"/>
       <c r="F73" s="5"/>
       <c r="G73" s="6"/>
-      <c r="H73" s="30"/>
-      <c r="I73" s="30"/>
-      <c r="J73" s="30"/>
-      <c r="K73" s="30"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="7" t="s">
@@ -2817,13 +2814,13 @@
       <c r="D74" s="29">
         <v>4974</v>
       </c>
-      <c r="E74" s="30"/>
+      <c r="E74" s="4"/>
       <c r="F74" s="5"/>
       <c r="G74" s="6"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="30"/>
-      <c r="J74" s="30"/>
-      <c r="K74" s="30"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="7" t="s">
@@ -2838,13 +2835,13 @@
       <c r="D75" s="29">
         <v>67</v>
       </c>
-      <c r="E75" s="30"/>
+      <c r="E75" s="4"/>
       <c r="F75" s="5"/>
       <c r="G75" s="6"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="7" t="s">
@@ -2859,13 +2856,13 @@
       <c r="D76" s="29">
         <v>232</v>
       </c>
-      <c r="E76" s="30"/>
+      <c r="E76" s="4"/>
       <c r="F76" s="5"/>
       <c r="G76" s="6"/>
-      <c r="H76" s="30"/>
-      <c r="I76" s="30"/>
-      <c r="J76" s="30"/>
-      <c r="K76" s="30"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="7" t="s">
@@ -2880,13 +2877,13 @@
       <c r="D77" s="29">
         <v>27</v>
       </c>
-      <c r="E77" s="30"/>
+      <c r="E77" s="4"/>
       <c r="F77" s="5"/>
       <c r="G77" s="6"/>
-      <c r="H77" s="30"/>
-      <c r="I77" s="30"/>
-      <c r="J77" s="30"/>
-      <c r="K77" s="30"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="7" t="s">
@@ -2901,13 +2898,13 @@
       <c r="D78" s="29">
         <v>51</v>
       </c>
-      <c r="E78" s="30"/>
+      <c r="E78" s="4"/>
       <c r="F78" s="5"/>
       <c r="G78" s="6"/>
-      <c r="H78" s="30"/>
-      <c r="I78" s="30"/>
-      <c r="J78" s="30"/>
-      <c r="K78" s="30"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="7" t="s">
@@ -2922,13 +2919,13 @@
       <c r="D79" s="29">
         <v>109</v>
       </c>
-      <c r="E79" s="30"/>
+      <c r="E79" s="4"/>
       <c r="F79" s="5"/>
       <c r="G79" s="6"/>
-      <c r="H79" s="30"/>
-      <c r="I79" s="30"/>
-      <c r="J79" s="30"/>
-      <c r="K79" s="30"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="7" t="s">
@@ -2943,13 +2940,13 @@
       <c r="D80" s="29">
         <v>55</v>
       </c>
-      <c r="E80" s="30"/>
+      <c r="E80" s="4"/>
       <c r="F80" s="5"/>
       <c r="G80" s="6"/>
-      <c r="H80" s="30"/>
-      <c r="I80" s="30"/>
-      <c r="J80" s="30"/>
-      <c r="K80" s="30"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="7" t="s">
@@ -2964,13 +2961,13 @@
       <c r="D81" s="29">
         <v>37</v>
       </c>
-      <c r="E81" s="30"/>
+      <c r="E81" s="4"/>
       <c r="F81" s="5"/>
       <c r="G81" s="6"/>
-      <c r="H81" s="30"/>
-      <c r="I81" s="30"/>
-      <c r="J81" s="30"/>
-      <c r="K81" s="30"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="7" t="s">
@@ -2985,19 +2982,19 @@
       <c r="D82" s="29">
         <v>74</v>
       </c>
-      <c r="E82" s="30"/>
+      <c r="E82" s="4"/>
       <c r="F82" s="5"/>
       <c r="G82" s="6"/>
-      <c r="H82" s="30"/>
-      <c r="I82" s="30"/>
-      <c r="J82" s="30"/>
-      <c r="K82" s="30"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="31" t="s">
+      <c r="B83" s="30" t="s">
         <v>165</v>
       </c>
       <c r="C83" s="29">
@@ -3006,13 +3003,13 @@
       <c r="D83" s="29">
         <v>154</v>
       </c>
-      <c r="E83" s="30"/>
+      <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="6"/>
-      <c r="H83" s="30"/>
-      <c r="I83" s="30"/>
-      <c r="J83" s="30"/>
-      <c r="K83" s="30"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="7" t="s">
@@ -3027,13 +3024,13 @@
       <c r="D84" s="29">
         <v>38</v>
       </c>
-      <c r="E84" s="30"/>
+      <c r="E84" s="4"/>
       <c r="F84" s="5"/>
       <c r="G84" s="6"/>
-      <c r="H84" s="30"/>
-      <c r="I84" s="30"/>
-      <c r="J84" s="30"/>
-      <c r="K84" s="30"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="7" t="s">
@@ -3048,13 +3045,13 @@
       <c r="D85" s="29">
         <v>529</v>
       </c>
-      <c r="E85" s="30"/>
+      <c r="E85" s="4"/>
       <c r="F85" s="5"/>
       <c r="G85" s="6"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="30"/>
-      <c r="J85" s="30"/>
-      <c r="K85" s="30"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="7" t="s">
@@ -3069,13 +3066,13 @@
       <c r="D86" s="29">
         <v>1671</v>
       </c>
-      <c r="E86" s="30"/>
+      <c r="E86" s="4"/>
       <c r="F86" s="5"/>
       <c r="G86" s="6"/>
-      <c r="H86" s="30"/>
-      <c r="I86" s="30"/>
-      <c r="J86" s="30"/>
-      <c r="K86" s="30"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="7" t="s">
@@ -3090,13 +3087,13 @@
       <c r="D87" s="29">
         <v>618</v>
       </c>
-      <c r="E87" s="30"/>
+      <c r="E87" s="4"/>
       <c r="F87" s="5"/>
       <c r="G87" s="6"/>
-      <c r="H87" s="30"/>
-      <c r="I87" s="30"/>
-      <c r="J87" s="30"/>
-      <c r="K87" s="30"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="7" t="s">
@@ -3111,13 +3108,13 @@
       <c r="D88" s="29">
         <v>194</v>
       </c>
-      <c r="E88" s="30"/>
+      <c r="E88" s="4"/>
       <c r="F88" s="5"/>
       <c r="G88" s="6"/>
-      <c r="H88" s="30"/>
-      <c r="I88" s="30"/>
-      <c r="J88" s="30"/>
-      <c r="K88" s="30"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="7" t="s">
@@ -3132,13 +3129,13 @@
       <c r="D89" s="29">
         <v>613</v>
       </c>
-      <c r="E89" s="30"/>
+      <c r="E89" s="4"/>
       <c r="F89" s="5"/>
       <c r="G89" s="6"/>
-      <c r="H89" s="30"/>
-      <c r="I89" s="30"/>
-      <c r="J89" s="30"/>
-      <c r="K89" s="30"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="7" t="s">
@@ -3153,13 +3150,13 @@
       <c r="D90" s="29">
         <v>1811</v>
       </c>
-      <c r="E90" s="30"/>
+      <c r="E90" s="4"/>
       <c r="F90" s="5"/>
       <c r="G90" s="6"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="30"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>